<commit_message>
Updated design documents and updated the language for step 1 in the 303 protocol if 3 fasting blood glucose measurements are not available.
</commit_message>
<xml_diff>
--- a/Design/UI/CollaboRhythm.Tablet/Insulin Titration Decision Support Text.xlsx
+++ b/Design/UI/CollaboRhythm.Tablet/Insulin Titration Decision Support Text.xlsx
@@ -688,9 +688,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>

</xml_diff>